<commit_message>
add tcl to the attention
</commit_message>
<xml_diff>
--- a/run_name.xlsx
+++ b/run_name.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.badzohreh\Desktop\university\swin github\001\tensorized_swin_transformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DABBE9-FDCC-4B42-B563-6532F82E5F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453640C2-D7A4-4CB8-9447-7DBF8B729330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BC9EC6D8-3C02-4C26-B296-CC6EE85B1941}"/>
   </bookViews>
@@ -574,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8227B274-9E33-42F0-9ADE-307457E422C3}">
   <dimension ref="A1:T68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
add tcl to the main code
</commit_message>
<xml_diff>
--- a/run_name.xlsx
+++ b/run_name.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.badzohreh\Desktop\university\swin github\001\tensorized_swin_transformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453640C2-D7A4-4CB8-9447-7DBF8B729330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47552317-43CB-4A2B-B706-8F023EE108E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BC9EC6D8-3C02-4C26-B296-CC6EE85B1941}"/>
   </bookViews>
@@ -574,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8227B274-9E33-42F0-9ADE-307457E422C3}">
   <dimension ref="A1:T68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>